<commit_message>
Updated the daily status tracker with latest info.
</commit_message>
<xml_diff>
--- a/docs/Daily Status Tracker.xlsx
+++ b/docs/Daily Status Tracker.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVWMigration\OVWMigration\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\OVW Migration Project\OVWMigration\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
-    <sheet name="Details" sheetId="1" r:id="rId2"/>
-    <sheet name="Pending URLs" sheetId="5" r:id="rId3"/>
+    <sheet name="Pending URLs" sheetId="5" r:id="rId2"/>
+    <sheet name="Details" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="114">
   <si>
     <t>URL</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t xml:space="preserve">The above number refer to the activities which are completed. Please go to next tab to check on the activities in progress. </t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Product-Listing</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -545,6 +551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -853,7 +860,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,16 +900,16 @@
         <v>95</v>
       </c>
       <c r="B4" s="16">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C4" s="16">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D4" s="16">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E4" s="16">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -940,11 +947,363 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="88.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="14"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="14"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="14"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A25" r:id="rId1"/>
+    <hyperlink ref="A24" r:id="rId2"/>
+    <hyperlink ref="A28" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
+    <hyperlink ref="A31" r:id="rId5"/>
+    <hyperlink ref="A14" r:id="rId6"/>
+    <hyperlink ref="A30" r:id="rId7"/>
+    <hyperlink ref="A13" r:id="rId8"/>
+    <hyperlink ref="A27" r:id="rId9"/>
+    <hyperlink ref="A5" r:id="rId10"/>
+    <hyperlink ref="A34" r:id="rId11"/>
+    <hyperlink ref="A36" r:id="rId12"/>
+    <hyperlink ref="A22" r:id="rId13"/>
+    <hyperlink ref="A19" r:id="rId14"/>
+    <hyperlink ref="A7" r:id="rId15"/>
+    <hyperlink ref="A37" r:id="rId16"/>
+    <hyperlink ref="A11" r:id="rId17"/>
+    <hyperlink ref="A21" r:id="rId18"/>
+    <hyperlink ref="A18" r:id="rId19"/>
+    <hyperlink ref="A29" r:id="rId20"/>
+    <hyperlink ref="A6" r:id="rId21"/>
+    <hyperlink ref="A35" r:id="rId22"/>
+    <hyperlink ref="A10" r:id="rId23"/>
+    <hyperlink ref="A32" r:id="rId24"/>
+    <hyperlink ref="A20" r:id="rId25"/>
+    <hyperlink ref="A17" r:id="rId26"/>
+    <hyperlink ref="A33" r:id="rId27"/>
+    <hyperlink ref="A8" r:id="rId28"/>
+    <hyperlink ref="A3" r:id="rId29"/>
+    <hyperlink ref="A2" r:id="rId30"/>
+    <hyperlink ref="A16" r:id="rId31"/>
+    <hyperlink ref="A23" r:id="rId32"/>
+    <hyperlink ref="A4" r:id="rId33"/>
+    <hyperlink ref="A38" r:id="rId34"/>
+    <hyperlink ref="A15" r:id="rId35"/>
+    <hyperlink ref="A12" r:id="rId36"/>
+    <hyperlink ref="A26" r:id="rId37"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1588,6 +1947,446 @@
       <c r="I21" s="22"/>
       <c r="J21" s="17">
         <v>42341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="14">
+        <v>48</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="14">
+        <v>48</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I23" s="22"/>
+      <c r="J23" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="14">
+        <v>48</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I24" s="22"/>
+      <c r="J24" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="14">
+        <v>48</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I25" s="22"/>
+      <c r="J25" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" s="14">
+        <v>48</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I26" s="22"/>
+      <c r="J26" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="14">
+        <v>48</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" s="22"/>
+      <c r="J27" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="14">
+        <v>48</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I28" s="22"/>
+      <c r="J28" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="14">
+        <v>48</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G29" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I29" s="22"/>
+      <c r="J29" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="14">
+        <v>48</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I30" s="22"/>
+      <c r="J30" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="17">
+        <v>42347</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D31" s="14">
+        <v>48</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="17">
+        <v>42345</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="14">
+        <v>48</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="I32" s="22"/>
+      <c r="J32" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="17">
+        <v>42347</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="14">
+        <v>48</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H33" s="13"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <v>42347</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="14">
+        <v>48</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" s="13"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
+        <v>42347</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="14">
+        <v>48</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H35" s="13"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="17">
+        <v>42349</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <v>42347</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="14">
+        <v>48</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="17">
+        <v>42349</v>
       </c>
     </row>
   </sheetData>
@@ -1611,466 +2410,22 @@
     <hyperlink ref="B4" r:id="rId17"/>
     <hyperlink ref="B3" r:id="rId18"/>
     <hyperlink ref="B6" r:id="rId19"/>
+    <hyperlink ref="B23" r:id="rId20"/>
+    <hyperlink ref="B22" r:id="rId21"/>
+    <hyperlink ref="B25" r:id="rId22"/>
+    <hyperlink ref="B24" r:id="rId23"/>
+    <hyperlink ref="B26" r:id="rId24"/>
+    <hyperlink ref="B28" r:id="rId25"/>
+    <hyperlink ref="B27" r:id="rId26"/>
+    <hyperlink ref="B29" r:id="rId27"/>
+    <hyperlink ref="B30" r:id="rId28"/>
+    <hyperlink ref="B32" r:id="rId29"/>
+    <hyperlink ref="B33" r:id="rId30"/>
+    <hyperlink ref="B35" r:id="rId31"/>
+    <hyperlink ref="B34" r:id="rId32"/>
+    <hyperlink ref="B36" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="88.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="11" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="14"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="14"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="14"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="14"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="14"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="14"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="14"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" s="14"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" s="14"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" s="14"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" s="14"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="14"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="14"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="14"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" s="14"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="14"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="14"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B52" s="14"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" s="14"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A30" r:id="rId1"/>
-    <hyperlink ref="A29" r:id="rId2"/>
-    <hyperlink ref="A44" r:id="rId3"/>
-    <hyperlink ref="A19" r:id="rId4"/>
-    <hyperlink ref="A33" r:id="rId5"/>
-    <hyperlink ref="A43" r:id="rId6"/>
-    <hyperlink ref="A9" r:id="rId7"/>
-    <hyperlink ref="A46" r:id="rId8"/>
-    <hyperlink ref="A37" r:id="rId9"/>
-    <hyperlink ref="A36" r:id="rId10"/>
-    <hyperlink ref="A38" r:id="rId11"/>
-    <hyperlink ref="A39" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
-    <hyperlink ref="A35" r:id="rId14"/>
-    <hyperlink ref="A13" r:id="rId15"/>
-    <hyperlink ref="A18" r:id="rId16"/>
-    <hyperlink ref="A32" r:id="rId17"/>
-    <hyperlink ref="A5" r:id="rId18"/>
-    <hyperlink ref="A42" r:id="rId19"/>
-    <hyperlink ref="A47" r:id="rId20"/>
-    <hyperlink ref="A27" r:id="rId21"/>
-    <hyperlink ref="A21" r:id="rId22"/>
-    <hyperlink ref="A7" r:id="rId23"/>
-    <hyperlink ref="A48" r:id="rId24"/>
-    <hyperlink ref="A11" r:id="rId25"/>
-    <hyperlink ref="A26" r:id="rId26"/>
-    <hyperlink ref="A20" r:id="rId27"/>
-    <hyperlink ref="A34" r:id="rId28"/>
-    <hyperlink ref="A6" r:id="rId29"/>
-    <hyperlink ref="A45" r:id="rId30"/>
-    <hyperlink ref="A10" r:id="rId31"/>
-    <hyperlink ref="A40" r:id="rId32"/>
-    <hyperlink ref="A25" r:id="rId33"/>
-    <hyperlink ref="A17" r:id="rId34"/>
-    <hyperlink ref="A41" r:id="rId35"/>
-    <hyperlink ref="A8" r:id="rId36"/>
-    <hyperlink ref="A23" r:id="rId37"/>
-    <hyperlink ref="A3" r:id="rId38"/>
-    <hyperlink ref="A50" r:id="rId39"/>
-    <hyperlink ref="A22" r:id="rId40"/>
-    <hyperlink ref="A2" r:id="rId41"/>
-    <hyperlink ref="A49" r:id="rId42"/>
-    <hyperlink ref="A24" r:id="rId43"/>
-    <hyperlink ref="A51" r:id="rId44"/>
-    <hyperlink ref="A16" r:id="rId45"/>
-    <hyperlink ref="A28" r:id="rId46"/>
-    <hyperlink ref="A4" r:id="rId47"/>
-    <hyperlink ref="A52" r:id="rId48"/>
-    <hyperlink ref="A15" r:id="rId49"/>
-    <hyperlink ref="A12" r:id="rId50"/>
-    <hyperlink ref="A31" r:id="rId51"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the tracker with the latest status.
</commit_message>
<xml_diff>
--- a/docs/Daily Status Tracker.xlsx
+++ b/docs/Daily Status Tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="114">
   <si>
     <t>URL</t>
   </si>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,10 +906,10 @@
         <v>35</v>
       </c>
       <c r="D4" s="16">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" s="16">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -949,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1620,7 @@
         <v>91</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I22" s="22"/>
       <c r="J22" s="17">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="I27" s="22"/>
       <c r="J27" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="I28" s="22"/>
       <c r="J28" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="I29" s="22"/>
       <c r="J29" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="I30" s="22"/>
       <c r="J30" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -1889,10 +1889,10 @@
       <c r="G31" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H31" s="13"/>
+      <c r="H31" s="14"/>
       <c r="I31" s="22"/>
       <c r="J31" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1920,7 +1920,7 @@
       <c r="H32" s="14"/>
       <c r="I32" s="22"/>
       <c r="J32" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1945,10 +1945,10 @@
       <c r="G33" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H33" s="13"/>
+      <c r="H33" s="14"/>
       <c r="I33" s="22"/>
       <c r="J33" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1971,12 +1971,14 @@
         <v>91</v>
       </c>
       <c r="G34" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H34" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H34" s="13"/>
       <c r="I34" s="22"/>
       <c r="J34" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1999,12 +2001,14 @@
         <v>91</v>
       </c>
       <c r="G35" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H35" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H35" s="13"/>
       <c r="I35" s="22"/>
       <c r="J35" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -2027,12 +2031,14 @@
         <v>91</v>
       </c>
       <c r="G36" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H36" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H36" s="13"/>
       <c r="I36" s="22"/>
       <c r="J36" s="17">
-        <v>42349</v>
+        <v>42353</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the document with latest info.
</commit_message>
<xml_diff>
--- a/docs/Daily Status Tracker.xlsx
+++ b/docs/Daily Status Tracker.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\OVW Migration Project\OVWMigration\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="114">
   <si>
     <t>URL</t>
   </si>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,16 +900,16 @@
         <v>95</v>
       </c>
       <c r="B4" s="16">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C4" s="16">
         <v>35</v>
       </c>
       <c r="D4" s="16">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E4" s="16">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -947,10 +947,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1452,7 +1452,7 @@
         <v>87</v>
       </c>
       <c r="D17" s="14">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>91</v>
@@ -1483,7 +1483,7 @@
         <v>87</v>
       </c>
       <c r="D18" s="14">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>91</v>
@@ -1514,7 +1514,7 @@
         <v>87</v>
       </c>
       <c r="D19" s="14">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>91</v>
@@ -1545,7 +1545,7 @@
         <v>87</v>
       </c>
       <c r="D20" s="14">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>91</v>
@@ -1578,7 +1578,7 @@
         <v>87</v>
       </c>
       <c r="D21" s="14">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>91</v>
@@ -1650,7 +1650,7 @@
         <v>91</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I23" s="22"/>
       <c r="J23" s="17">
@@ -1710,7 +1710,7 @@
         <v>91</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I25" s="22"/>
       <c r="J25" s="17">
@@ -1740,7 +1740,7 @@
         <v>91</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I26" s="22"/>
       <c r="J26" s="17">
@@ -1770,7 +1770,7 @@
         <v>91</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I27" s="22"/>
       <c r="J27" s="17">
@@ -1800,7 +1800,7 @@
         <v>91</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I28" s="22"/>
       <c r="J28" s="17">
@@ -1830,7 +1830,7 @@
         <v>91</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I29" s="22"/>
       <c r="J29" s="17">
@@ -1860,7 +1860,7 @@
         <v>91</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I30" s="22"/>
       <c r="J30" s="17">
@@ -1887,9 +1887,11 @@
         <v>91</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H31" s="14"/>
+        <v>91</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="I31" s="22"/>
       <c r="J31" s="17">
         <v>42353</v>
@@ -1915,9 +1917,11 @@
         <v>91</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H32" s="14"/>
+        <v>91</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="I32" s="22"/>
       <c r="J32" s="17">
         <v>42353</v>
@@ -1943,9 +1947,11 @@
         <v>91</v>
       </c>
       <c r="G33" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H33" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="H33" s="14"/>
       <c r="I33" s="22"/>
       <c r="J33" s="17">
         <v>42353</v>
@@ -2039,6 +2045,198 @@
       <c r="I36" s="22"/>
       <c r="J36" s="17">
         <v>42353</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
+        <v>42352</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="14">
+        <v>9</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H37" s="13"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="17">
+        <v>42356</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
+        <v>42352</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="14">
+        <v>9</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H38" s="13"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="17">
+        <v>42356</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
+        <v>42352</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="14">
+        <v>9</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="17">
+        <v>42356</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
+        <v>42352</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="14">
+        <v>9</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H40" s="13"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="17">
+        <v>42356</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="17">
+        <v>42352</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="14">
+        <v>9</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G41" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H41" s="13"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="17">
+        <v>42356</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
+        <v>42352</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="14">
+        <v>9</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="H42" s="13"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="17">
+        <v>42356</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>42352</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="14">
+        <v>9</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="17">
+        <v>42356</v>
       </c>
     </row>
   </sheetData>
@@ -2076,17 +2274,26 @@
     <hyperlink ref="B35" r:id="rId31"/>
     <hyperlink ref="B34" r:id="rId32"/>
     <hyperlink ref="B36" r:id="rId33"/>
+    <hyperlink ref="B42" r:id="rId34"/>
+    <hyperlink ref="B41" r:id="rId35"/>
+    <hyperlink ref="B43" r:id="rId36"/>
+    <hyperlink ref="B40" r:id="rId37"/>
+    <hyperlink ref="B37" r:id="rId38"/>
+    <hyperlink ref="B38" r:id="rId39"/>
+    <hyperlink ref="B39" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId34"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2095,342 +2302,271 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>90</v>
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>24</v>
+      <c r="A8" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>36</v>
+      <c r="A14" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>43</v>
+      <c r="A19" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>87</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>88</v>
-      </c>
+      <c r="A24" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="14"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>58</v>
+      <c r="A26" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>89</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B28" s="14"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="14"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="14"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B38" s="14"/>
+      <c r="B30" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A25" r:id="rId1"/>
-    <hyperlink ref="A24" r:id="rId2"/>
-    <hyperlink ref="A28" r:id="rId3"/>
-    <hyperlink ref="A9" r:id="rId4"/>
-    <hyperlink ref="A31" r:id="rId5"/>
-    <hyperlink ref="A14" r:id="rId6"/>
-    <hyperlink ref="A30" r:id="rId7"/>
-    <hyperlink ref="A13" r:id="rId8"/>
-    <hyperlink ref="A27" r:id="rId9"/>
-    <hyperlink ref="A5" r:id="rId10"/>
-    <hyperlink ref="A34" r:id="rId11"/>
-    <hyperlink ref="A36" r:id="rId12"/>
-    <hyperlink ref="A22" r:id="rId13"/>
-    <hyperlink ref="A19" r:id="rId14"/>
-    <hyperlink ref="A7" r:id="rId15"/>
-    <hyperlink ref="A37" r:id="rId16"/>
-    <hyperlink ref="A11" r:id="rId17"/>
+    <hyperlink ref="A18" r:id="rId1"/>
+    <hyperlink ref="A17" r:id="rId2"/>
+    <hyperlink ref="A23" r:id="rId3"/>
+    <hyperlink ref="A8" r:id="rId4"/>
+    <hyperlink ref="A22" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A20" r:id="rId7"/>
+    <hyperlink ref="A1" r:id="rId8"/>
+    <hyperlink ref="A26" r:id="rId9"/>
+    <hyperlink ref="A28" r:id="rId10"/>
+    <hyperlink ref="A16" r:id="rId11"/>
+    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A3" r:id="rId13"/>
+    <hyperlink ref="A29" r:id="rId14"/>
+    <hyperlink ref="A6" r:id="rId15"/>
+    <hyperlink ref="A15" r:id="rId16"/>
+    <hyperlink ref="A12" r:id="rId17"/>
     <hyperlink ref="A21" r:id="rId18"/>
-    <hyperlink ref="A18" r:id="rId19"/>
-    <hyperlink ref="A29" r:id="rId20"/>
-    <hyperlink ref="A6" r:id="rId21"/>
-    <hyperlink ref="A35" r:id="rId22"/>
-    <hyperlink ref="A10" r:id="rId23"/>
-    <hyperlink ref="A32" r:id="rId24"/>
-    <hyperlink ref="A20" r:id="rId25"/>
-    <hyperlink ref="A17" r:id="rId26"/>
-    <hyperlink ref="A33" r:id="rId27"/>
-    <hyperlink ref="A8" r:id="rId28"/>
-    <hyperlink ref="A3" r:id="rId29"/>
-    <hyperlink ref="A2" r:id="rId30"/>
-    <hyperlink ref="A16" r:id="rId31"/>
-    <hyperlink ref="A23" r:id="rId32"/>
-    <hyperlink ref="A4" r:id="rId33"/>
-    <hyperlink ref="A38" r:id="rId34"/>
-    <hyperlink ref="A15" r:id="rId35"/>
-    <hyperlink ref="A12" r:id="rId36"/>
-    <hyperlink ref="A26" r:id="rId37"/>
+    <hyperlink ref="A2" r:id="rId19"/>
+    <hyperlink ref="A27" r:id="rId20"/>
+    <hyperlink ref="A5" r:id="rId21"/>
+    <hyperlink ref="A24" r:id="rId22"/>
+    <hyperlink ref="A14" r:id="rId23"/>
+    <hyperlink ref="A11" r:id="rId24"/>
+    <hyperlink ref="A25" r:id="rId25"/>
+    <hyperlink ref="A4" r:id="rId26"/>
+    <hyperlink ref="A10" r:id="rId27"/>
+    <hyperlink ref="A30" r:id="rId28"/>
+    <hyperlink ref="A9" r:id="rId29"/>
+    <hyperlink ref="A19" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with the latest details.
</commit_message>
<xml_diff>
--- a/docs/Daily Status Tracker.xlsx
+++ b/docs/Daily Status Tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\OVW Migration Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="117">
   <si>
     <t>URL</t>
   </si>
@@ -363,6 +363,15 @@
   </si>
   <si>
     <t>Product-Listing</t>
+  </si>
+  <si>
+    <t>Resp-B.Guide</t>
+  </si>
+  <si>
+    <t>Buyers-Guide</t>
+  </si>
+  <si>
+    <t>In Progress(9 locales testing completed, rest in progress)</t>
   </si>
 </sst>
 </file>
@@ -860,7 +869,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,16 +909,16 @@
         <v>95</v>
       </c>
       <c r="B4" s="16">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C4" s="16">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D4" s="16">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E4" s="16">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -947,10 +956,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +969,7 @@
     <col min="3" max="3" width="17.28515625" style="11" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="11" customWidth="1"/>
     <col min="5" max="7" width="17.140625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="52.28515625" style="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.140625" style="10" customWidth="1"/>
     <col min="10" max="10" width="17.140625" style="11" customWidth="1"/>
     <col min="12" max="12" width="17.140625" customWidth="1"/>
@@ -1017,7 +1026,7 @@
         <v>91</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="25"/>
@@ -1950,7 +1959,7 @@
         <v>91</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I33" s="22"/>
       <c r="J33" s="17">
@@ -1980,7 +1989,7 @@
         <v>91</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I34" s="22"/>
       <c r="J34" s="17">
@@ -2010,7 +2019,7 @@
         <v>91</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I35" s="22"/>
       <c r="J35" s="17">
@@ -2040,7 +2049,7 @@
         <v>91</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="I36" s="22"/>
       <c r="J36" s="17">
@@ -2058,21 +2067,23 @@
         <v>87</v>
       </c>
       <c r="D37" s="14">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H37" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>116</v>
+      </c>
       <c r="I37" s="22"/>
       <c r="J37" s="17">
-        <v>42356</v>
+        <v>42360</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2086,21 +2097,23 @@
         <v>83</v>
       </c>
       <c r="D38" s="14">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H38" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>116</v>
+      </c>
       <c r="I38" s="22"/>
       <c r="J38" s="17">
-        <v>42356</v>
+        <v>42360</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2114,19 +2127,23 @@
         <v>83</v>
       </c>
       <c r="D39" s="14">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>116</v>
+      </c>
       <c r="I39" s="22"/>
       <c r="J39" s="17">
-        <v>42356</v>
+        <v>42360</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2140,21 +2157,23 @@
         <v>89</v>
       </c>
       <c r="D40" s="14">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H40" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="I40" s="22"/>
       <c r="J40" s="17">
-        <v>42356</v>
+        <v>42360</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2168,21 +2187,23 @@
         <v>81</v>
       </c>
       <c r="D41" s="14">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H41" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>116</v>
+      </c>
       <c r="I41" s="22"/>
       <c r="J41" s="17">
-        <v>42356</v>
+        <v>42360</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2196,21 +2217,23 @@
         <v>81</v>
       </c>
       <c r="D42" s="14">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="H42" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>116</v>
+      </c>
       <c r="I42" s="22"/>
       <c r="J42" s="17">
-        <v>42356</v>
+        <v>42360</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2224,20 +2247,67 @@
         <v>81</v>
       </c>
       <c r="D43" s="14">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E43" s="14" t="s">
         <v>91</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>116</v>
+      </c>
       <c r="I43" s="22"/>
       <c r="J43" s="17">
+        <v>42360</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
         <v>42356</v>
       </c>
+      <c r="B44" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D44" s="14">
+        <v>9</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="17">
+        <v>42356</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D45" s="14">
+        <v>9</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D50" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2281,18 +2351,20 @@
     <hyperlink ref="B37" r:id="rId38"/>
     <hyperlink ref="B38" r:id="rId39"/>
     <hyperlink ref="B39" r:id="rId40"/>
+    <hyperlink ref="B44" r:id="rId41"/>
+    <hyperlink ref="B45" r:id="rId42"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId41"/>
+  <pageSetup orientation="portrait" r:id="rId43"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2327,7 +2399,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>83</v>
@@ -2335,7 +2407,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>83</v>
@@ -2343,47 +2415,47 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>35</v>
+      <c r="A7" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>36</v>
+      <c r="A8" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>86</v>
@@ -2391,23 +2463,23 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>87</v>
@@ -2415,23 +2487,23 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>56</v>
+      <c r="A17" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>88</v>
@@ -2439,61 +2511,63 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>58</v>
+      <c r="A19" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>62</v>
+      <c r="A22" s="8" t="s">
+        <v>67</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="14"/>
+      <c r="A24" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>113</v>
@@ -2501,15 +2575,15 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>113</v>
@@ -2517,56 +2591,42 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="14"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="14"/>
+      <c r="B28" s="14" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A18" r:id="rId1"/>
-    <hyperlink ref="A17" r:id="rId2"/>
-    <hyperlink ref="A23" r:id="rId3"/>
-    <hyperlink ref="A8" r:id="rId4"/>
-    <hyperlink ref="A22" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A20" r:id="rId7"/>
+    <hyperlink ref="A16" r:id="rId1"/>
+    <hyperlink ref="A15" r:id="rId2"/>
+    <hyperlink ref="A21" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4"/>
+    <hyperlink ref="A20" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A18" r:id="rId7"/>
     <hyperlink ref="A1" r:id="rId8"/>
-    <hyperlink ref="A26" r:id="rId9"/>
-    <hyperlink ref="A28" r:id="rId10"/>
-    <hyperlink ref="A16" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
+    <hyperlink ref="A24" r:id="rId9"/>
+    <hyperlink ref="A26" r:id="rId10"/>
+    <hyperlink ref="A14" r:id="rId11"/>
+    <hyperlink ref="A11" r:id="rId12"/>
     <hyperlink ref="A3" r:id="rId13"/>
-    <hyperlink ref="A29" r:id="rId14"/>
-    <hyperlink ref="A6" r:id="rId15"/>
-    <hyperlink ref="A15" r:id="rId16"/>
-    <hyperlink ref="A12" r:id="rId17"/>
-    <hyperlink ref="A21" r:id="rId18"/>
+    <hyperlink ref="A27" r:id="rId14"/>
+    <hyperlink ref="A5" r:id="rId15"/>
+    <hyperlink ref="A13" r:id="rId16"/>
+    <hyperlink ref="A10" r:id="rId17"/>
+    <hyperlink ref="A19" r:id="rId18"/>
     <hyperlink ref="A2" r:id="rId19"/>
-    <hyperlink ref="A27" r:id="rId20"/>
-    <hyperlink ref="A5" r:id="rId21"/>
-    <hyperlink ref="A24" r:id="rId22"/>
-    <hyperlink ref="A14" r:id="rId23"/>
-    <hyperlink ref="A11" r:id="rId24"/>
-    <hyperlink ref="A25" r:id="rId25"/>
-    <hyperlink ref="A4" r:id="rId26"/>
-    <hyperlink ref="A10" r:id="rId27"/>
-    <hyperlink ref="A30" r:id="rId28"/>
-    <hyperlink ref="A9" r:id="rId29"/>
-    <hyperlink ref="A19" r:id="rId30"/>
+    <hyperlink ref="A25" r:id="rId20"/>
+    <hyperlink ref="A4" r:id="rId21"/>
+    <hyperlink ref="A22" r:id="rId22"/>
+    <hyperlink ref="A12" r:id="rId23"/>
+    <hyperlink ref="A9" r:id="rId24"/>
+    <hyperlink ref="A23" r:id="rId25"/>
+    <hyperlink ref="A8" r:id="rId26"/>
+    <hyperlink ref="A28" r:id="rId27"/>
+    <hyperlink ref="A17" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update the daily status tracker.
</commit_message>
<xml_diff>
--- a/docs/Daily Status Tracker.xlsx
+++ b/docs/Daily Status Tracker.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\OVW Migration Project\Daily Checkout\4 Jan\OVWMigration\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\OVW Migration Project\Daily Checkout\8 Jan\OVWMigration\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="161">
   <si>
     <t>URL</t>
   </si>
@@ -481,9 +481,6 @@
     <t>Redirected page</t>
   </si>
   <si>
-    <t>Page is not available across all locales.</t>
-  </si>
-  <si>
     <t>Waiting for node structure</t>
   </si>
   <si>
@@ -506,6 +503,9 @@
   </si>
   <si>
     <t>Partners</t>
+  </si>
+  <si>
+    <t>Redirected page (new)</t>
   </si>
 </sst>
 </file>
@@ -994,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,10 +1035,10 @@
         <v>95</v>
       </c>
       <c r="B4" s="13">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C4" s="13">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D4" s="13">
         <v>61</v>
@@ -1082,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1193,7 @@
       <c r="K3" s="27"/>
       <c r="L3" s="23"/>
       <c r="M3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1217,7 +1217,7 @@
         <v>91</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I4" s="26"/>
       <c r="J4" s="14">
@@ -2230,7 +2230,7 @@
         <v>91</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I37" s="24"/>
       <c r="J37" s="14">
@@ -2261,7 +2261,7 @@
         <v>91</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I38" s="24"/>
       <c r="J38" s="14">
@@ -2292,7 +2292,7 @@
         <v>91</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I39" s="24"/>
       <c r="J39" s="14">
@@ -2323,7 +2323,7 @@
         <v>91</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I40" s="24"/>
       <c r="J40" s="14">
@@ -2354,7 +2354,7 @@
         <v>91</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I41" s="24"/>
       <c r="J41" s="14">
@@ -2385,7 +2385,7 @@
         <v>91</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I42" s="24"/>
       <c r="J42" s="14">
@@ -2416,7 +2416,7 @@
         <v>91</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I43" s="24"/>
       <c r="J43" s="14">
@@ -2447,7 +2447,7 @@
         <v>91</v>
       </c>
       <c r="H44" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I44" s="24"/>
       <c r="J44" s="14">
@@ -2478,7 +2478,7 @@
         <v>91</v>
       </c>
       <c r="H45" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I45" s="24"/>
       <c r="J45" s="14">
@@ -2509,7 +2509,7 @@
         <v>91</v>
       </c>
       <c r="H46" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I46" s="24"/>
       <c r="J46" s="14">
@@ -2540,7 +2540,7 @@
         <v>91</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I47" s="24"/>
       <c r="J47" s="14">
@@ -2571,7 +2571,7 @@
         <v>91</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I48" s="24"/>
       <c r="J48" s="14">
@@ -2602,7 +2602,7 @@
         <v>91</v>
       </c>
       <c r="H49" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I49" s="24"/>
       <c r="J49" s="14">
@@ -2633,7 +2633,7 @@
         <v>91</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I50" s="24"/>
       <c r="J50" s="14">
@@ -2691,7 +2691,7 @@
         <v>91</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I52" s="24"/>
       <c r="J52" s="14">
@@ -2722,7 +2722,7 @@
         <v>91</v>
       </c>
       <c r="H53" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I53" s="24"/>
       <c r="J53" s="14">
@@ -2753,7 +2753,7 @@
         <v>91</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I54" s="24"/>
       <c r="J54" s="14">
@@ -2876,7 +2876,7 @@
         <v>91</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I58" s="24"/>
       <c r="J58" s="14">
@@ -2936,7 +2936,7 @@
         <v>91</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I60" s="24"/>
       <c r="J60" s="14">
@@ -3022,7 +3022,7 @@
         <v>91</v>
       </c>
       <c r="H63" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I63" s="24"/>
       <c r="J63" s="14">
@@ -3067,7 +3067,7 @@
         <v>122</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D65" s="11">
         <v>9</v>
@@ -3082,7 +3082,7 @@
         <v>91</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I65" s="24"/>
       <c r="J65" s="14">
@@ -3097,7 +3097,7 @@
         <v>126</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D66" s="11">
         <v>9</v>
@@ -3115,6 +3115,62 @@
       <c r="I66" s="25"/>
       <c r="J66" s="14">
         <v>42380</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="14">
+        <v>42011</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" s="11">
+        <v>9</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H67" s="11"/>
+      <c r="I67" s="25"/>
+      <c r="J67" s="14">
+        <v>42382</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" s="14">
+        <v>42011</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="D68" s="11">
+        <v>9</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F68" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="H68" s="11"/>
+      <c r="I68" s="25"/>
+      <c r="J68" s="14">
+        <v>42382</v>
       </c>
     </row>
   </sheetData>
@@ -3181,15 +3237,17 @@
     <hyperlink ref="B64" r:id="rId60"/>
     <hyperlink ref="B65" r:id="rId61"/>
     <hyperlink ref="B66" r:id="rId62"/>
+    <hyperlink ref="B68" r:id="rId63"/>
+    <hyperlink ref="B67" r:id="rId64"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId63"/>
+  <pageSetup orientation="portrait" r:id="rId65"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3268,296 +3326,274 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>88</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>152</v>
+        <v>120</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="25" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>88</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="B9" s="11"/>
       <c r="C9" s="6" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="25" t="s">
-        <v>108</v>
+      <c r="C10" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B34" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>117</v>
+      </c>
       <c r="C34" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B38" s="6">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="B39" s="6">
-        <v>6</v>
+      <c r="B36" s="6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="6">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3565,41 +3601,39 @@
     <hyperlink ref="A5" r:id="rId1"/>
     <hyperlink ref="A6" r:id="rId2"/>
     <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="A8" r:id="rId4"/>
-    <hyperlink ref="A7" r:id="rId5"/>
-    <hyperlink ref="A9" r:id="rId6"/>
-    <hyperlink ref="A3" r:id="rId7"/>
-    <hyperlink ref="A4" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A26" r:id="rId10"/>
+    <hyperlink ref="A3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="A8" r:id="rId6"/>
+    <hyperlink ref="A24" r:id="rId7"/>
+    <hyperlink ref="A20" r:id="rId8"/>
+    <hyperlink ref="A21" r:id="rId9"/>
+    <hyperlink ref="A23" r:id="rId10"/>
     <hyperlink ref="A22" r:id="rId11"/>
-    <hyperlink ref="A23" r:id="rId12"/>
-    <hyperlink ref="A25" r:id="rId13"/>
-    <hyperlink ref="A24" r:id="rId14"/>
-    <hyperlink ref="A21" r:id="rId15"/>
-    <hyperlink ref="A16" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
-    <hyperlink ref="A17" r:id="rId19"/>
-    <hyperlink ref="A14" r:id="rId20"/>
-    <hyperlink ref="A13" r:id="rId21"/>
-    <hyperlink ref="A33" r:id="rId22"/>
-    <hyperlink ref="A28" r:id="rId23"/>
-    <hyperlink ref="A12" r:id="rId24"/>
-    <hyperlink ref="A15" r:id="rId25"/>
-    <hyperlink ref="A11" r:id="rId26"/>
-    <hyperlink ref="A35" r:id="rId27"/>
-    <hyperlink ref="A31" r:id="rId28"/>
-    <hyperlink ref="A20" r:id="rId29"/>
-    <hyperlink ref="A27" r:id="rId30"/>
+    <hyperlink ref="A19" r:id="rId12"/>
+    <hyperlink ref="A14" r:id="rId13"/>
+    <hyperlink ref="A16" r:id="rId14"/>
+    <hyperlink ref="A17" r:id="rId15"/>
+    <hyperlink ref="A15" r:id="rId16"/>
+    <hyperlink ref="A12" r:id="rId17"/>
+    <hyperlink ref="A11" r:id="rId18"/>
+    <hyperlink ref="A31" r:id="rId19"/>
+    <hyperlink ref="A26" r:id="rId20"/>
+    <hyperlink ref="A10" r:id="rId21"/>
+    <hyperlink ref="A13" r:id="rId22"/>
+    <hyperlink ref="A9" r:id="rId23"/>
+    <hyperlink ref="A33" r:id="rId24"/>
+    <hyperlink ref="A29" r:id="rId25"/>
+    <hyperlink ref="A18" r:id="rId26"/>
+    <hyperlink ref="A25" r:id="rId27"/>
+    <hyperlink ref="A30" r:id="rId28"/>
+    <hyperlink ref="A27" r:id="rId29"/>
+    <hyperlink ref="A28" r:id="rId30"/>
     <hyperlink ref="A32" r:id="rId31"/>
-    <hyperlink ref="A29" r:id="rId32"/>
-    <hyperlink ref="A30" r:id="rId33"/>
-    <hyperlink ref="A34" r:id="rId34"/>
-    <hyperlink ref="A36" r:id="rId35"/>
+    <hyperlink ref="A34" r:id="rId32"/>
+    <hyperlink ref="A7" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId36"/>
+  <pageSetup orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated the daily status tracker and added the OVW Demo Wave 1 Batch 1 document.
</commit_message>
<xml_diff>
--- a/docs/Daily Status Tracker.xlsx
+++ b/docs/Daily Status Tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rdevalka\OVW Migration Project\Daily Checkout\29 Jan\OVWMigration\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,14 +19,14 @@
     <sheet name="Final URLs" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Details!$A$1:$M$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Details!$A$1:$M$93</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="170">
   <si>
     <t>URL</t>
   </si>
@@ -472,9 +472,6 @@
     <t>Additional Comments</t>
   </si>
   <si>
-    <t>Out of Scope</t>
-  </si>
-  <si>
     <t>Redirected page</t>
   </si>
   <si>
@@ -511,15 +508,9 @@
     <t>9 locales test to start</t>
   </si>
   <si>
-    <t>48 locales testing in progress</t>
-  </si>
-  <si>
     <t>Reports shared for test</t>
   </si>
   <si>
-    <t>9 locales re-test</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -535,25 +526,16 @@
     <t>9 locales test in progress</t>
   </si>
   <si>
-    <t>Web URLs testing status</t>
-  </si>
-  <si>
     <t>Support</t>
   </si>
   <si>
-    <t>48 locales tested with issues.</t>
-  </si>
-  <si>
-    <t>48 locales testing done</t>
-  </si>
-  <si>
-    <t>48 locales tested with issues</t>
-  </si>
-  <si>
-    <t>9 locales re-test to start</t>
-  </si>
-  <si>
-    <t>9 locales tested with issues</t>
+    <t>Testing completed for 9 locales.</t>
+  </si>
+  <si>
+    <t>9 locales test done</t>
+  </si>
+  <si>
+    <t>Testing completed today for 9 locales with issues</t>
   </si>
 </sst>
 </file>
@@ -672,7 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -711,9 +693,6 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -723,7 +702,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -746,6 +724,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1055,7 +1036,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,13 +1049,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1090,10 +1071,10 @@
         <v>4</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="F3" s="27" t="s">
         <v>154</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1101,64 +1082,64 @@
         <v>95</v>
       </c>
       <c r="B4" s="13">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C4" s="13">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D4" s="13">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E4" s="13">
-        <v>84</v>
-      </c>
-      <c r="F4" s="28">
+        <v>88</v>
+      </c>
+      <c r="F4" s="26">
         <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I6" s="31" t="s">
-        <v>165</v>
+      <c r="I6" s="29" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="I7" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="J7" s="31">
-        <v>65</v>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="I7" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="J7" s="29">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="I8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J8">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="I9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J9">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1166,7 +1147,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1177,82 +1158,50 @@
         <v>168</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E14" s="29"/>
+      <c r="E14" s="27"/>
       <c r="I14" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="J16" s="31">
+      <c r="I16" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="J16" s="29">
         <f>SUM(J8:J14)</f>
-        <v>65</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I18" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="J18" s="31">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I19" t="s">
-        <v>175</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="20" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I20" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
+      <c r="I20" s="30"/>
     </row>
     <row r="21" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I21" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="J21">
-        <v>5</v>
-      </c>
+      <c r="I21" s="30"/>
     </row>
     <row r="22" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I22" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="J22">
-        <v>11</v>
-      </c>
+      <c r="I22" s="30"/>
     </row>
     <row r="23" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I23" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="J23">
-        <v>3</v>
-      </c>
+      <c r="I23" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1274,16 +1223,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M91"/>
+  <dimension ref="A1:M93"/>
   <sheetViews>
-    <sheetView topLeftCell="C64" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="87.7109375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="87.7109375" style="18" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="8" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="8" customWidth="1"/>
     <col min="5" max="7" width="17.140625" style="7" customWidth="1"/>
@@ -1328,7 +1277,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -1349,15 +1298,15 @@
       <c r="H2" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="23"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="14">
         <v>42374</v>
       </c>
-      <c r="K2" s="26"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="11" t="s">
@@ -1378,19 +1327,19 @@
       <c r="H3" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I3" s="23"/>
+      <c r="I3" s="34"/>
       <c r="J3" s="14">
         <v>42374</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="23"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="22"/>
       <c r="M3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="11" t="s">
@@ -1408,22 +1357,22 @@
       <c r="G4" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" s="23"/>
+      <c r="H4" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" s="34"/>
       <c r="J4" s="14">
         <v>42374</v>
       </c>
-      <c r="K4" s="26"/>
-      <c r="L4" s="21"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="20"/>
       <c r="M4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -1444,19 +1393,19 @@
       <c r="H5" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="34"/>
       <c r="J5" s="14">
         <v>42374</v>
       </c>
-      <c r="K5" s="26"/>
-      <c r="L5" s="20"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="19"/>
       <c r="M5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="12" t="s">
@@ -1477,7 +1426,7 @@
       <c r="H6" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I6" s="18"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="14">
         <v>42341</v>
       </c>
@@ -1488,7 +1437,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -1509,7 +1458,7 @@
       <c r="H7" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I7" s="18"/>
+      <c r="I7" s="34"/>
       <c r="J7" s="14">
         <v>42341</v>
       </c>
@@ -1520,7 +1469,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="21" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="12" t="s">
@@ -1541,7 +1490,7 @@
       <c r="H8" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I8" s="18"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="14">
         <v>42341</v>
       </c>
@@ -1552,7 +1501,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="12" t="s">
@@ -1573,14 +1522,14 @@
       <c r="H9" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="18"/>
+      <c r="I9" s="34"/>
       <c r="J9" s="14">
         <v>42341</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="12" t="s">
@@ -1601,14 +1550,14 @@
       <c r="H10" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="18"/>
+      <c r="I10" s="34"/>
       <c r="J10" s="14">
         <v>42341</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="12" t="s">
@@ -1629,7 +1578,7 @@
       <c r="H11" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I11" s="18"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="14">
         <v>42341</v>
       </c>
@@ -1639,7 +1588,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -1660,7 +1609,7 @@
       <c r="H12" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="18"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="14">
         <v>42341</v>
       </c>
@@ -1670,7 +1619,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="12" t="s">
@@ -1691,7 +1640,7 @@
       <c r="H13" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="18"/>
+      <c r="I13" s="34"/>
       <c r="J13" s="14">
         <v>42341</v>
       </c>
@@ -1701,7 +1650,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -1722,7 +1671,7 @@
       <c r="H14" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I14" s="18"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="14">
         <v>42341</v>
       </c>
@@ -1732,7 +1681,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="12" t="s">
@@ -1753,7 +1702,7 @@
       <c r="H15" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="18"/>
+      <c r="I15" s="34"/>
       <c r="J15" s="14">
         <v>42341</v>
       </c>
@@ -1763,7 +1712,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C16" s="12" t="s">
@@ -1784,7 +1733,7 @@
       <c r="H16" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I16" s="18"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="14">
         <v>42341</v>
       </c>
@@ -1794,7 +1743,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -1815,7 +1764,7 @@
       <c r="H17" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I17" s="18"/>
+      <c r="I17" s="34"/>
       <c r="J17" s="14">
         <v>42341</v>
       </c>
@@ -1827,7 +1776,7 @@
       <c r="A18" s="14">
         <v>42341</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="21" t="s">
         <v>54</v>
       </c>
       <c r="C18" s="12" t="s">
@@ -1848,7 +1797,7 @@
       <c r="H18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="18"/>
+      <c r="I18" s="34"/>
       <c r="J18" s="14">
         <v>42341</v>
       </c>
@@ -1860,7 +1809,7 @@
       <c r="A19" s="14">
         <v>42345</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C19" s="12" t="s">
@@ -1881,7 +1830,7 @@
       <c r="H19" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I19" s="18"/>
+      <c r="I19" s="34"/>
       <c r="J19" s="14">
         <v>42349</v>
       </c>
@@ -1893,7 +1842,7 @@
       <c r="A20" s="14">
         <v>42345</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="21" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="12" t="s">
@@ -1914,7 +1863,7 @@
       <c r="H20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="18"/>
+      <c r="I20" s="34"/>
       <c r="J20" s="14">
         <v>42349</v>
       </c>
@@ -1926,7 +1875,7 @@
       <c r="A21" s="14">
         <v>42345</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="21" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="12" t="s">
@@ -1947,7 +1896,7 @@
       <c r="H21" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I21" s="18"/>
+      <c r="I21" s="34"/>
       <c r="J21" s="14">
         <v>42349</v>
       </c>
@@ -1956,7 +1905,7 @@
       <c r="A22" s="14">
         <v>42345</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="21" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="12" t="s">
@@ -1977,7 +1926,7 @@
       <c r="H22" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I22" s="18"/>
+      <c r="I22" s="34"/>
       <c r="J22" s="14">
         <v>42349</v>
       </c>
@@ -1986,7 +1935,7 @@
       <c r="A23" s="14">
         <v>42345</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="21" t="s">
         <v>63</v>
       </c>
       <c r="C23" s="12" t="s">
@@ -2007,7 +1956,7 @@
       <c r="H23" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="18"/>
+      <c r="I23" s="34"/>
       <c r="J23" s="14">
         <v>42353</v>
       </c>
@@ -2016,7 +1965,7 @@
       <c r="A24" s="14">
         <v>42345</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="21" t="s">
         <v>64</v>
       </c>
       <c r="C24" s="12" t="s">
@@ -2037,7 +1986,7 @@
       <c r="H24" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I24" s="18"/>
+      <c r="I24" s="34"/>
       <c r="J24" s="14">
         <v>42353</v>
       </c>
@@ -2046,7 +1995,7 @@
       <c r="A25" s="14">
         <v>42345</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="21" t="s">
         <v>65</v>
       </c>
       <c r="C25" s="12" t="s">
@@ -2067,7 +2016,7 @@
       <c r="H25" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I25" s="18"/>
+      <c r="I25" s="34"/>
       <c r="J25" s="14">
         <v>42353</v>
       </c>
@@ -2076,7 +2025,7 @@
       <c r="A26" s="14">
         <v>42345</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="21" t="s">
         <v>73</v>
       </c>
       <c r="C26" s="12" t="s">
@@ -2097,7 +2046,7 @@
       <c r="H26" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I26" s="18"/>
+      <c r="I26" s="34"/>
       <c r="J26" s="14">
         <v>42353</v>
       </c>
@@ -2106,7 +2055,7 @@
       <c r="A27" s="14">
         <v>42347</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="21" t="s">
         <v>80</v>
       </c>
       <c r="C27" s="12" t="s">
@@ -2127,7 +2076,7 @@
       <c r="H27" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I27" s="18"/>
+      <c r="I27" s="34"/>
       <c r="J27" s="14">
         <v>42353</v>
       </c>
@@ -2136,7 +2085,7 @@
       <c r="A28" s="14">
         <v>42347</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="21" t="s">
         <v>76</v>
       </c>
       <c r="C28" s="12" t="s">
@@ -2157,7 +2106,7 @@
       <c r="H28" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I28" s="18"/>
+      <c r="I28" s="34"/>
       <c r="J28" s="14">
         <v>42353</v>
       </c>
@@ -2166,7 +2115,7 @@
       <c r="A29" s="14">
         <v>42347</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="21" t="s">
         <v>77</v>
       </c>
       <c r="C29" s="12" t="s">
@@ -2187,7 +2136,7 @@
       <c r="H29" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I29" s="18"/>
+      <c r="I29" s="34"/>
       <c r="J29" s="14">
         <v>42353</v>
       </c>
@@ -2196,7 +2145,7 @@
       <c r="A30" s="14">
         <v>42347</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="21" t="s">
         <v>78</v>
       </c>
       <c r="C30" s="12" t="s">
@@ -2217,7 +2166,7 @@
       <c r="H30" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I30" s="18"/>
+      <c r="I30" s="34"/>
       <c r="J30" s="14">
         <v>42353</v>
       </c>
@@ -2226,7 +2175,7 @@
       <c r="A31" s="14">
         <v>42352</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="21" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="12" t="s">
@@ -2247,7 +2196,7 @@
       <c r="H31" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I31" s="24"/>
+      <c r="I31" s="23"/>
       <c r="J31" s="14">
         <v>42360</v>
       </c>
@@ -2256,7 +2205,7 @@
       <c r="A32" s="14">
         <v>42352</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="12" t="s">
@@ -2277,7 +2226,7 @@
       <c r="H32" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I32" s="24"/>
+      <c r="I32" s="23"/>
       <c r="J32" s="14">
         <v>42360</v>
       </c>
@@ -2286,7 +2235,7 @@
       <c r="A33" s="14">
         <v>42352</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="21" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="12" t="s">
@@ -2307,7 +2256,7 @@
       <c r="H33" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I33" s="18"/>
+      <c r="I33" s="34"/>
       <c r="J33" s="14">
         <v>42360</v>
       </c>
@@ -2316,7 +2265,7 @@
       <c r="A34" s="14">
         <v>42352</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="21" t="s">
         <v>10</v>
       </c>
       <c r="C34" s="12" t="s">
@@ -2337,7 +2286,7 @@
       <c r="H34" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I34" s="18"/>
+      <c r="I34" s="34"/>
       <c r="J34" s="14">
         <v>42360</v>
       </c>
@@ -2346,7 +2295,7 @@
       <c r="A35" s="14">
         <v>42352</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="21" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="12" t="s">
@@ -2367,7 +2316,7 @@
       <c r="H35" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I35" s="24"/>
+      <c r="I35" s="23"/>
       <c r="J35" s="14">
         <v>42360</v>
       </c>
@@ -2376,7 +2325,7 @@
       <c r="A36" s="14">
         <v>42356</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="21" t="s">
         <v>37</v>
       </c>
       <c r="C36" s="12" t="s">
@@ -2392,24 +2341,26 @@
         <v>91</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="25"/>
+        <v>91</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I36" s="23"/>
       <c r="J36" s="14"/>
-      <c r="K36" s="26"/>
+      <c r="K36" s="24"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="14">
         <v>42356</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="21" t="s">
         <v>24</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D37" s="30">
+      <c r="D37" s="28">
         <v>9</v>
       </c>
       <c r="E37" s="11" t="s">
@@ -2422,25 +2373,25 @@
         <v>91</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="I37" s="24"/>
+        <v>91</v>
+      </c>
+      <c r="I37" s="23"/>
       <c r="J37" s="14">
         <v>42375</v>
       </c>
-      <c r="K37" s="26"/>
+      <c r="K37" s="24"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="14">
         <v>42359</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="30">
+      <c r="D38" s="28">
         <v>9</v>
       </c>
       <c r="E38" s="11" t="s">
@@ -2453,25 +2404,25 @@
         <v>91</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="I38" s="24"/>
+        <v>91</v>
+      </c>
+      <c r="I38" s="23"/>
       <c r="J38" s="14">
         <v>42375</v>
       </c>
-      <c r="K38" s="26"/>
+      <c r="K38" s="24"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="14">
         <v>42359</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D39" s="30">
+      <c r="D39" s="28">
         <v>9</v>
       </c>
       <c r="E39" s="11" t="s">
@@ -2484,25 +2435,25 @@
         <v>91</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="I39" s="24"/>
+        <v>91</v>
+      </c>
+      <c r="I39" s="23"/>
       <c r="J39" s="14">
         <v>42375</v>
       </c>
-      <c r="K39" s="26"/>
+      <c r="K39" s="24"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="14">
         <v>42359</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D40" s="30">
+      <c r="D40" s="28">
         <v>9</v>
       </c>
       <c r="E40" s="11" t="s">
@@ -2515,25 +2466,25 @@
         <v>91</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="I40" s="24"/>
+        <v>91</v>
+      </c>
+      <c r="I40" s="23"/>
       <c r="J40" s="14">
         <v>42375</v>
       </c>
-      <c r="K40" s="26"/>
+      <c r="K40" s="24"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="14">
         <v>42359</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="30">
+      <c r="D41" s="28">
         <v>9</v>
       </c>
       <c r="E41" s="11" t="s">
@@ -2546,19 +2497,19 @@
         <v>91</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>161</v>
-      </c>
-      <c r="I41" s="24"/>
+        <v>91</v>
+      </c>
+      <c r="I41" s="23"/>
       <c r="J41" s="14">
         <v>42375</v>
       </c>
-      <c r="K41" s="26"/>
+      <c r="K41" s="24"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="14">
         <v>42359</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="21" t="s">
         <v>68</v>
       </c>
       <c r="C42" s="12" t="s">
@@ -2579,17 +2530,17 @@
       <c r="H42" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I42" s="24"/>
+      <c r="I42" s="23"/>
       <c r="J42" s="14">
         <v>42375</v>
       </c>
-      <c r="K42" s="26"/>
+      <c r="K42" s="24"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="14">
         <v>42359</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="21" t="s">
         <v>72</v>
       </c>
       <c r="C43" s="12" t="s">
@@ -2610,17 +2561,17 @@
       <c r="H43" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I43" s="24"/>
+      <c r="I43" s="23"/>
       <c r="J43" s="14">
         <v>42375</v>
       </c>
-      <c r="K43" s="26"/>
+      <c r="K43" s="24"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="14">
         <v>42359</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="21" t="s">
         <v>75</v>
       </c>
       <c r="C44" s="12" t="s">
@@ -2641,17 +2592,17 @@
       <c r="H44" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I44" s="24"/>
+      <c r="I44" s="23"/>
       <c r="J44" s="14">
         <v>42375</v>
       </c>
-      <c r="K44" s="26"/>
+      <c r="K44" s="24"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="14">
         <v>42359</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="21" t="s">
         <v>39</v>
       </c>
       <c r="C45" s="12" t="s">
@@ -2672,17 +2623,17 @@
       <c r="H45" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I45" s="24"/>
+      <c r="I45" s="23"/>
       <c r="J45" s="14">
         <v>42375</v>
       </c>
-      <c r="K45" s="26"/>
+      <c r="K45" s="24"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="14">
         <v>42359</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="21" t="s">
         <v>42</v>
       </c>
       <c r="C46" s="12" t="s">
@@ -2703,17 +2654,17 @@
       <c r="H46" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I46" s="24"/>
+      <c r="I46" s="23"/>
       <c r="J46" s="14">
         <v>42375</v>
       </c>
-      <c r="K46" s="26"/>
+      <c r="K46" s="24"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="14">
         <v>42359</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="21" t="s">
         <v>43</v>
       </c>
       <c r="C47" s="12" t="s">
@@ -2734,17 +2685,17 @@
       <c r="H47" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I47" s="24"/>
+      <c r="I47" s="23"/>
       <c r="J47" s="14">
         <v>42375</v>
       </c>
-      <c r="K47" s="26"/>
+      <c r="K47" s="24"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="14">
         <v>42359</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="21" t="s">
         <v>47</v>
       </c>
       <c r="C48" s="12" t="s">
@@ -2765,17 +2716,17 @@
       <c r="H48" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I48" s="24"/>
+      <c r="I48" s="23"/>
       <c r="J48" s="14">
         <v>42375</v>
       </c>
-      <c r="K48" s="26"/>
+      <c r="K48" s="24"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="14">
         <v>42359</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="21" t="s">
         <v>50</v>
       </c>
       <c r="C49" s="12" t="s">
@@ -2796,17 +2747,17 @@
       <c r="H49" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I49" s="24"/>
+      <c r="I49" s="23"/>
       <c r="J49" s="14">
         <v>42375</v>
       </c>
-      <c r="K49" s="26"/>
+      <c r="K49" s="24"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="14">
         <v>42359</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="21" t="s">
         <v>51</v>
       </c>
       <c r="C50" s="12" t="s">
@@ -2827,17 +2778,17 @@
       <c r="H50" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I50" s="24"/>
+      <c r="I50" s="23"/>
       <c r="J50" s="14">
         <v>42375</v>
       </c>
-      <c r="K50" s="26"/>
+      <c r="K50" s="24"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="14">
         <v>42366</v>
       </c>
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="21" t="s">
         <v>38</v>
       </c>
       <c r="C51" s="11" t="s">
@@ -2853,18 +2804,20 @@
         <v>91</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H51" s="10"/>
-      <c r="I51" s="10"/>
+        <v>91</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I51" s="34"/>
       <c r="J51" s="11"/>
-      <c r="K51" s="26"/>
+      <c r="K51" s="24"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="14">
         <v>42367</v>
       </c>
-      <c r="B52" s="22" t="s">
+      <c r="B52" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C52" s="11" t="s">
@@ -2885,17 +2838,17 @@
       <c r="H52" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I52" s="24"/>
+      <c r="I52" s="23"/>
       <c r="J52" s="14">
         <v>42375</v>
       </c>
-      <c r="K52" s="26"/>
+      <c r="K52" s="24"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="14">
         <v>42367</v>
       </c>
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="21" t="s">
         <v>74</v>
       </c>
       <c r="C53" s="11" t="s">
@@ -2916,17 +2869,17 @@
       <c r="H53" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I53" s="24"/>
+      <c r="I53" s="23"/>
       <c r="J53" s="14">
         <v>42375</v>
       </c>
-      <c r="K53" s="26"/>
+      <c r="K53" s="24"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="14">
         <v>42368</v>
       </c>
-      <c r="B54" s="22" t="s">
+      <c r="B54" s="21" t="s">
         <v>79</v>
       </c>
       <c r="C54" s="11" t="s">
@@ -2947,17 +2900,17 @@
       <c r="H54" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I54" s="24"/>
+      <c r="I54" s="23"/>
       <c r="J54" s="14">
         <v>42375</v>
       </c>
-      <c r="K54" s="26"/>
+      <c r="K54" s="24"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="14">
         <v>42367</v>
       </c>
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="21" t="s">
         <v>62</v>
       </c>
       <c r="C55" s="11" t="s">
@@ -2978,17 +2931,17 @@
       <c r="H55" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I55" s="24"/>
+      <c r="I55" s="23"/>
       <c r="J55" s="14">
         <v>42375</v>
       </c>
-      <c r="K55" s="26"/>
+      <c r="K55" s="24"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="14">
         <v>42367</v>
       </c>
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="21" t="s">
         <v>66</v>
       </c>
       <c r="C56" s="11" t="s">
@@ -3009,17 +2962,17 @@
       <c r="H56" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I56" s="24"/>
+      <c r="I56" s="23"/>
       <c r="J56" s="14">
         <v>42375</v>
       </c>
-      <c r="K56" s="26"/>
+      <c r="K56" s="24"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="14">
         <v>42009</v>
       </c>
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="21" t="s">
         <v>13</v>
       </c>
       <c r="C57" s="12" t="s">
@@ -3040,7 +2993,7 @@
       <c r="H57" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I57" s="24"/>
+      <c r="I57" s="23"/>
       <c r="J57" s="14">
         <v>42377</v>
       </c>
@@ -3049,13 +3002,13 @@
       <c r="A58" s="14">
         <v>42009</v>
       </c>
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="21" t="s">
         <v>27</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D58" s="30">
+      <c r="D58" s="28">
         <v>48</v>
       </c>
       <c r="E58" s="11" t="s">
@@ -3070,7 +3023,7 @@
       <c r="H58" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I58" s="24"/>
+      <c r="I58" s="23"/>
       <c r="J58" s="14">
         <v>42377</v>
       </c>
@@ -3079,7 +3032,7 @@
       <c r="A59" s="14">
         <v>42009</v>
       </c>
-      <c r="B59" s="22" t="s">
+      <c r="B59" s="21" t="s">
         <v>49</v>
       </c>
       <c r="C59" s="12" t="s">
@@ -3100,7 +3053,7 @@
       <c r="H59" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I59" s="24"/>
+      <c r="I59" s="23"/>
       <c r="J59" s="14">
         <v>42377</v>
       </c>
@@ -3109,13 +3062,13 @@
       <c r="A60" s="14">
         <v>42009</v>
       </c>
-      <c r="B60" s="22" t="s">
+      <c r="B60" s="21" t="s">
         <v>41</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D60" s="30">
+      <c r="D60" s="28">
         <v>48</v>
       </c>
       <c r="E60" s="11" t="s">
@@ -3130,7 +3083,7 @@
       <c r="H60" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I60" s="24"/>
+      <c r="I60" s="23"/>
       <c r="J60" s="14">
         <v>42377</v>
       </c>
@@ -3139,7 +3092,7 @@
       <c r="A61" s="14">
         <v>42009</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="21" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="12" t="s">
@@ -3169,7 +3122,7 @@
       <c r="A62" s="14">
         <v>42009</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="21" t="s">
         <v>71</v>
       </c>
       <c r="C62" s="12" t="s">
@@ -3190,7 +3143,7 @@
       <c r="H62" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I62" s="23"/>
+      <c r="I62" s="24"/>
       <c r="J62" s="14">
         <v>42380</v>
       </c>
@@ -3199,13 +3152,13 @@
       <c r="A63" s="14">
         <v>42009</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="21" t="s">
         <v>26</v>
       </c>
       <c r="C63" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D63" s="30">
+      <c r="D63" s="28">
         <v>48</v>
       </c>
       <c r="E63" s="11" t="s">
@@ -3220,7 +3173,7 @@
       <c r="H63" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I63" s="24"/>
+      <c r="I63" s="23"/>
       <c r="J63" s="14">
         <v>42377</v>
       </c>
@@ -3229,7 +3182,7 @@
       <c r="A64" s="14">
         <v>42009</v>
       </c>
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="21" t="s">
         <v>60</v>
       </c>
       <c r="C64" s="12" t="s">
@@ -3250,7 +3203,7 @@
       <c r="H64" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I64" s="24"/>
+      <c r="I64" s="23"/>
       <c r="J64" s="14">
         <v>42377</v>
       </c>
@@ -3259,11 +3212,11 @@
       <c r="A65" s="14">
         <v>42009</v>
       </c>
-      <c r="B65" s="22" t="s">
+      <c r="B65" s="21" t="s">
         <v>121</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D65" s="11">
         <v>48</v>
@@ -3280,7 +3233,7 @@
       <c r="H65" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I65" s="24"/>
+      <c r="I65" s="23"/>
       <c r="J65" s="14">
         <v>42377</v>
       </c>
@@ -3289,11 +3242,11 @@
       <c r="A66" s="14">
         <v>42009</v>
       </c>
-      <c r="B66" s="22" t="s">
+      <c r="B66" s="21" t="s">
         <v>125</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D66" s="11">
         <v>48</v>
@@ -3310,7 +3263,7 @@
       <c r="H66" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I66" s="23"/>
+      <c r="I66" s="24"/>
       <c r="J66" s="14">
         <v>42380</v>
       </c>
@@ -3319,7 +3272,7 @@
       <c r="A67" s="14">
         <v>42011</v>
       </c>
-      <c r="B67" s="22" t="s">
+      <c r="B67" s="21" t="s">
         <v>56</v>
       </c>
       <c r="C67" s="11" t="s">
@@ -3340,7 +3293,7 @@
       <c r="H67" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I67" s="25"/>
+      <c r="I67" s="23"/>
       <c r="J67" s="14">
         <v>42382</v>
       </c>
@@ -3349,7 +3302,7 @@
       <c r="A68" s="14">
         <v>42011</v>
       </c>
-      <c r="B68" s="22" t="s">
+      <c r="B68" s="21" t="s">
         <v>57</v>
       </c>
       <c r="C68" s="11" t="s">
@@ -3370,7 +3323,7 @@
       <c r="H68" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="I68" s="25"/>
+      <c r="I68" s="23"/>
       <c r="J68" s="14">
         <v>42382</v>
       </c>
@@ -3379,11 +3332,11 @@
       <c r="A69" s="14">
         <v>42015</v>
       </c>
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="21" t="s">
         <v>120</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D69" s="11">
         <v>9</v>
@@ -3398,18 +3351,20 @@
         <v>91</v>
       </c>
       <c r="H69" s="11" t="s">
-        <v>161</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I69" s="23"/>
+      <c r="J69" s="23"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="14">
         <v>42015</v>
       </c>
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="21" t="s">
         <v>128</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D70" s="11">
         <v>9</v>
@@ -3424,21 +3379,23 @@
         <v>91</v>
       </c>
       <c r="H70" s="11" t="s">
-        <v>91</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I70" s="23"/>
+      <c r="J70" s="23"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="14">
         <v>42015</v>
       </c>
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="21" t="s">
         <v>129</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D71" s="11">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>91</v>
@@ -3450,21 +3407,23 @@
         <v>91</v>
       </c>
       <c r="H71" s="11" t="s">
-        <v>91</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I71" s="23"/>
+      <c r="J71" s="23"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="14">
         <v>42015</v>
       </c>
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="21" t="s">
         <v>134</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D72" s="11">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>91</v>
@@ -3476,21 +3435,23 @@
         <v>91</v>
       </c>
       <c r="H72" s="11" t="s">
-        <v>171</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I72" s="23"/>
+      <c r="J72" s="23"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="14">
         <v>42015</v>
       </c>
-      <c r="B73" s="22" t="s">
+      <c r="B73" s="21" t="s">
         <v>139</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D73" s="11">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E73" s="11" t="s">
         <v>91</v>
@@ -3502,18 +3463,20 @@
         <v>91</v>
       </c>
       <c r="H73" s="11" t="s">
-        <v>91</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I73" s="23"/>
+      <c r="J73" s="23"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="14">
         <v>42015</v>
       </c>
-      <c r="B74" s="22" t="s">
+      <c r="B74" s="21" t="s">
         <v>131</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D74" s="11">
         <v>9</v>
@@ -3528,18 +3491,20 @@
         <v>91</v>
       </c>
       <c r="H74" s="11" t="s">
-        <v>91</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I74" s="23"/>
+      <c r="J74" s="23"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="14">
         <v>42015</v>
       </c>
-      <c r="B75" s="22" t="s">
+      <c r="B75" s="21" t="s">
         <v>140</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D75" s="11">
         <v>9</v>
@@ -3554,18 +3519,20 @@
         <v>91</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>161</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I75" s="23"/>
+      <c r="J75" s="23"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="14">
         <v>42015</v>
       </c>
-      <c r="B76" s="22" t="s">
+      <c r="B76" s="21" t="s">
         <v>145</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D76" s="11">
         <v>9</v>
@@ -3580,18 +3547,20 @@
         <v>91</v>
       </c>
       <c r="H76" s="11" t="s">
-        <v>161</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I76" s="23"/>
+      <c r="J76" s="23"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="14">
         <v>42015</v>
       </c>
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="21" t="s">
         <v>143</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D77" s="11">
         <v>9</v>
@@ -3606,42 +3575,48 @@
         <v>91</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>171</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I77" s="23"/>
+      <c r="J77" s="23"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="14">
         <v>42015</v>
       </c>
-      <c r="B78" s="22" t="s">
+      <c r="B78" s="21" t="s">
         <v>122</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D78" s="11">
         <v>9</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H78" s="11"/>
+        <v>91</v>
+      </c>
+      <c r="H78" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="I78" s="23"/>
+      <c r="J78" s="23"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="14">
         <v>42016</v>
       </c>
-      <c r="B79" s="22" t="s">
+      <c r="B79" s="21" t="s">
         <v>141</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D79" s="11">
         <v>9</v>
@@ -3656,18 +3631,20 @@
         <v>91</v>
       </c>
       <c r="H79" s="11" t="s">
-        <v>161</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="I79" s="23"/>
+      <c r="J79" s="23"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="14">
         <v>42016</v>
       </c>
-      <c r="B80" s="22" t="s">
+      <c r="B80" s="21" t="s">
         <v>142</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D80" s="11">
         <v>9</v>
@@ -3682,18 +3659,20 @@
         <v>91</v>
       </c>
       <c r="H80" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I80" s="23"/>
+      <c r="J80" s="23"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="14">
         <v>42016</v>
       </c>
-      <c r="B81" s="22" t="s">
+      <c r="B81" s="21" t="s">
         <v>144</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D81" s="11">
         <v>9</v>
@@ -3708,18 +3687,20 @@
         <v>91</v>
       </c>
       <c r="H81" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I81" s="23"/>
+      <c r="J81" s="23"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="14">
         <v>42016</v>
       </c>
-      <c r="B82" s="22" t="s">
+      <c r="B82" s="21" t="s">
         <v>123</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D82" s="11">
         <v>9</v>
@@ -3734,21 +3715,23 @@
         <v>91</v>
       </c>
       <c r="H82" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I82" s="23"/>
+      <c r="J82" s="23"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="14">
         <v>42016</v>
       </c>
-      <c r="B83" s="22" t="s">
+      <c r="B83" s="21" t="s">
         <v>130</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D83" s="11">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E83" s="11" t="s">
         <v>91</v>
@@ -3760,18 +3743,20 @@
         <v>91</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I83" s="23"/>
+      <c r="J83" s="23"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="14">
         <v>42017</v>
       </c>
-      <c r="B84" s="22" t="s">
+      <c r="B84" s="21" t="s">
         <v>126</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D84" s="11">
         <v>9</v>
@@ -3786,18 +3771,20 @@
         <v>91</v>
       </c>
       <c r="H84" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I84" s="23"/>
+      <c r="J84" s="23"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="14">
         <v>42017</v>
       </c>
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="21" t="s">
         <v>127</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D85" s="11">
         <v>9</v>
@@ -3812,18 +3799,20 @@
         <v>91</v>
       </c>
       <c r="H85" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I85" s="23"/>
+      <c r="J85" s="23"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="14">
         <v>42017</v>
       </c>
-      <c r="B86" s="22" t="s">
+      <c r="B86" s="21" t="s">
         <v>132</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D86" s="11">
         <v>9</v>
@@ -3838,18 +3827,20 @@
         <v>91</v>
       </c>
       <c r="H86" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I86" s="23"/>
+      <c r="J86" s="23"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="14">
         <v>42017</v>
       </c>
-      <c r="B87" s="22" t="s">
+      <c r="B87" s="21" t="s">
         <v>136</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D87" s="11">
         <v>9</v>
@@ -3864,18 +3855,20 @@
         <v>91</v>
       </c>
       <c r="H87" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I87" s="23"/>
+      <c r="J87" s="23"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="14">
         <v>42017</v>
       </c>
-      <c r="B88" s="22" t="s">
+      <c r="B88" s="21" t="s">
         <v>133</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D88" s="11">
         <v>9</v>
@@ -3890,14 +3883,16 @@
         <v>91</v>
       </c>
       <c r="H88" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="I88" s="23"/>
+      <c r="J88" s="23"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="14">
         <v>42024</v>
       </c>
-      <c r="B89" s="22" t="s">
+      <c r="B89" s="21" t="s">
         <v>58</v>
       </c>
       <c r="C89" s="11" t="s">
@@ -3916,16 +3911,18 @@
         <v>91</v>
       </c>
       <c r="H89" s="10"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="23"/>
+      <c r="J89" s="23"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="14">
         <v>42024</v>
       </c>
-      <c r="B90" s="22" t="s">
+      <c r="B90" s="21" t="s">
         <v>119</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D90" s="11">
         <v>9</v>
@@ -3940,33 +3937,95 @@
         <v>110</v>
       </c>
       <c r="H90" s="10"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="23"/>
+      <c r="J90" s="23"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="14">
-        <v>42024</v>
-      </c>
-      <c r="B91" s="22" t="s">
-        <v>138</v>
+        <v>42029</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>12</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>166</v>
+        <v>82</v>
       </c>
       <c r="D91" s="11">
         <v>9</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H91" s="10"/>
+        <v>91</v>
+      </c>
+      <c r="H91" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="I91" s="23"/>
+      <c r="J91" s="23"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="14">
+        <v>42029</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D92" s="11">
+        <v>9</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F92" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H92" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="I92" s="23"/>
+      <c r="J92" s="23"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="14">
+        <v>42029</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D93" s="11">
+        <v>9</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H93" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="I93" s="23"/>
+      <c r="J93" s="23"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M91"/>
+  <autoFilter ref="A1:M93"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
@@ -4055,19 +4114,19 @@
     <hyperlink ref="B90" r:id="rId85"/>
     <hyperlink ref="B89" r:id="rId86"/>
     <hyperlink ref="B91" r:id="rId87"/>
+    <hyperlink ref="B92" r:id="rId88"/>
+    <hyperlink ref="B93" r:id="rId89"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId88"/>
+  <pageSetup orientation="portrait" r:id="rId90"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4088,146 +4147,119 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
-        <v>12</v>
+      <c r="A2" s="21" t="s">
+        <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>82</v>
+        <v>117</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>89</v>
+      <c r="A3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>69</v>
+      <c r="A4" s="21" t="s">
+        <v>16</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>14</v>
+      <c r="A5" s="21" t="s">
+        <v>118</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="23"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C6" s="23"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C8" s="25"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C9" s="25"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>149</v>
+      <c r="B11" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="6">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B13" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B14" s="6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="33"/>
-      <c r="B15" s="5"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1"/>
-    <hyperlink ref="A7" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="A10" r:id="rId6"/>
-    <hyperlink ref="A9" r:id="rId7"/>
-    <hyperlink ref="A8" r:id="rId8"/>
-    <hyperlink ref="A11" r:id="rId9"/>
-    <hyperlink ref="A6" r:id="rId10"/>
+    <hyperlink ref="A8" r:id="rId1"/>
+    <hyperlink ref="A6" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
+    <hyperlink ref="A7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -4246,7 +4278,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="12" t="s">
@@ -4254,7 +4286,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -4262,7 +4294,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="12" t="s">
@@ -4270,7 +4302,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -4278,7 +4310,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -4286,7 +4318,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>71</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -4294,7 +4326,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -4302,7 +4334,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -4310,75 +4342,75 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>122</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>140</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>145</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>122</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>141</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>142</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>144</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>133</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>131</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -4419,7 +4451,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="21" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -4427,7 +4459,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
@@ -4435,7 +4467,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="11" t="s">
@@ -4443,7 +4475,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -4451,7 +4483,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -4459,7 +4491,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>57</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -4467,7 +4499,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -4475,7 +4507,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="21" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -4483,7 +4515,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="21" t="s">
         <v>62</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -4491,7 +4523,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="21" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -4499,7 +4531,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -4507,7 +4539,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="21" t="s">
         <v>69</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -4515,7 +4547,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="21" t="s">
         <v>74</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -4523,7 +4555,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>79</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -4531,7 +4563,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -4539,7 +4571,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -4547,7 +4579,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -4555,7 +4587,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="12" t="s">
@@ -4563,7 +4595,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="12" t="s">
@@ -4571,7 +4603,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -4579,7 +4611,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="21" t="s">
         <v>21</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -4587,7 +4619,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="21" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="12" t="s">
@@ -4595,7 +4627,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="21" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="12" t="s">
@@ -4603,7 +4635,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="21" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -4611,7 +4643,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="12" t="s">
@@ -4619,7 +4651,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -4627,7 +4659,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="21" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="12" t="s">
@@ -4635,7 +4667,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -4643,7 +4675,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="21" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -4651,7 +4683,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="21" t="s">
         <v>48</v>
       </c>
       <c r="B30" s="12" t="s">
@@ -4659,7 +4691,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="21" t="s">
         <v>49</v>
       </c>
       <c r="B31" s="12" t="s">
@@ -4667,7 +4699,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="21" t="s">
         <v>52</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -4675,7 +4707,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="21" t="s">
         <v>53</v>
       </c>
       <c r="B33" s="12" t="s">
@@ -4683,7 +4715,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="21" t="s">
         <v>54</v>
       </c>
       <c r="B34" s="12" t="s">
@@ -4691,7 +4723,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="21" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="12" t="s">
@@ -4699,7 +4731,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="22" t="s">
+      <c r="A36" s="21" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="12" t="s">
@@ -4707,7 +4739,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="21" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="12" t="s">
@@ -4715,7 +4747,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="21" t="s">
         <v>45</v>
       </c>
       <c r="B38" s="12" t="s">
@@ -4723,7 +4755,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="A39" s="21" t="s">
         <v>46</v>
       </c>
       <c r="B39" s="12" t="s">
@@ -4731,7 +4763,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
+      <c r="A40" s="21" t="s">
         <v>63</v>
       </c>
       <c r="B40" s="12" t="s">
@@ -4739,7 +4771,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
+      <c r="A41" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B41" s="12" t="s">
@@ -4747,7 +4779,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="21" t="s">
         <v>65</v>
       </c>
       <c r="B42" s="12" t="s">
@@ -4755,7 +4787,7 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
+      <c r="A43" s="21" t="s">
         <v>73</v>
       </c>
       <c r="B43" s="12" t="s">
@@ -4763,7 +4795,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
+      <c r="A44" s="21" t="s">
         <v>80</v>
       </c>
       <c r="B44" s="12" t="s">
@@ -4771,7 +4803,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B45" s="12" t="s">
@@ -4779,7 +4811,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="21" t="s">
         <v>71</v>
       </c>
       <c r="B46" s="12" t="s">
@@ -4787,7 +4819,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
+      <c r="A47" s="21" t="s">
         <v>76</v>
       </c>
       <c r="B47" s="12" t="s">
@@ -4795,7 +4827,7 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
+      <c r="A48" s="21" t="s">
         <v>77</v>
       </c>
       <c r="B48" s="12" t="s">
@@ -4803,7 +4835,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
+      <c r="A49" s="21" t="s">
         <v>78</v>
       </c>
       <c r="B49" s="12" t="s">
@@ -4811,7 +4843,7 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
+      <c r="A50" s="21" t="s">
         <v>55</v>
       </c>
       <c r="B50" s="12" t="s">
@@ -4819,7 +4851,7 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
+      <c r="A51" s="21" t="s">
         <v>26</v>
       </c>
       <c r="B51" s="12" t="s">
@@ -4827,7 +4859,7 @@
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
+      <c r="A52" s="21" t="s">
         <v>33</v>
       </c>
       <c r="B52" s="12" t="s">
@@ -4835,7 +4867,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
+      <c r="A53" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B53" s="12" t="s">
@@ -4843,7 +4875,7 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="22" t="s">
+      <c r="A54" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B54" s="12" t="s">
@@ -4851,7 +4883,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
+      <c r="A55" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B55" s="12" t="s">
@@ -4859,7 +4891,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B56" s="12" t="s">
@@ -4867,7 +4899,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="21" t="s">
         <v>37</v>
       </c>
       <c r="B57" s="12" t="s">
@@ -4875,7 +4907,7 @@
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
+      <c r="A58" s="21" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="12" t="s">
@@ -4883,7 +4915,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
+      <c r="A59" s="21" t="s">
         <v>28</v>
       </c>
       <c r="B59" s="12" t="s">
@@ -4891,7 +4923,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
+      <c r="A60" s="21" t="s">
         <v>29</v>
       </c>
       <c r="B60" s="12" t="s">
@@ -4899,7 +4931,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="22" t="s">
+      <c r="A61" s="21" t="s">
         <v>35</v>
       </c>
       <c r="B61" s="12" t="s">
@@ -4907,7 +4939,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
+      <c r="A62" s="21" t="s">
         <v>36</v>
       </c>
       <c r="B62" s="12" t="s">
@@ -4915,7 +4947,7 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="22" t="s">
+      <c r="A63" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B63" s="12" t="s">
@@ -4923,7 +4955,7 @@
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="22" t="s">
+      <c r="A64" s="21" t="s">
         <v>72</v>
       </c>
       <c r="B64" s="12" t="s">
@@ -4931,7 +4963,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="22" t="s">
+      <c r="A65" s="21" t="s">
         <v>75</v>
       </c>
       <c r="B65" s="12" t="s">
@@ -4939,7 +4971,7 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="22" t="s">
+      <c r="A66" s="21" t="s">
         <v>39</v>
       </c>
       <c r="B66" s="12" t="s">
@@ -4947,7 +4979,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="22" t="s">
+      <c r="A67" s="21" t="s">
         <v>42</v>
       </c>
       <c r="B67" s="12" t="s">
@@ -4955,7 +4987,7 @@
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="22" t="s">
+      <c r="A68" s="21" t="s">
         <v>43</v>
       </c>
       <c r="B68" s="12" t="s">
@@ -4963,7 +4995,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="22" t="s">
+      <c r="A69" s="21" t="s">
         <v>47</v>
       </c>
       <c r="B69" s="12" t="s">
@@ -4971,7 +5003,7 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="22" t="s">
+      <c r="A70" s="21" t="s">
         <v>50</v>
       </c>
       <c r="B70" s="12" t="s">
@@ -4979,7 +5011,7 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="22" t="s">
+      <c r="A71" s="21" t="s">
         <v>51</v>
       </c>
       <c r="B71" s="12" t="s">
@@ -4987,7 +5019,7 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="22" t="s">
+      <c r="A72" s="21" t="s">
         <v>61</v>
       </c>
       <c r="B72" s="12" t="s">
@@ -4995,169 +5027,169 @@
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="22" t="s">
+      <c r="A73" s="21" t="s">
         <v>118</v>
       </c>
       <c r="B73" s="11"/>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="22" t="s">
+      <c r="A74" s="21" t="s">
         <v>119</v>
       </c>
       <c r="B74" s="11"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="22" t="s">
+      <c r="A75" s="21" t="s">
         <v>120</v>
       </c>
       <c r="B75" s="11"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="22" t="s">
+      <c r="A76" s="21" t="s">
         <v>121</v>
       </c>
       <c r="B76" s="11"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="22" t="s">
+      <c r="A77" s="21" t="s">
         <v>122</v>
       </c>
       <c r="B77" s="11"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="22" t="s">
+      <c r="A78" s="21" t="s">
         <v>123</v>
       </c>
       <c r="B78" s="11"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="22" t="s">
+      <c r="A79" s="21" t="s">
         <v>124</v>
       </c>
       <c r="B79" s="11"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="22" t="s">
+      <c r="A80" s="21" t="s">
         <v>125</v>
       </c>
       <c r="B80" s="11"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="22" t="s">
+      <c r="A81" s="21" t="s">
         <v>126</v>
       </c>
       <c r="B81" s="11"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="22" t="s">
+      <c r="A82" s="21" t="s">
         <v>127</v>
       </c>
       <c r="B82" s="11"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="22" t="s">
+      <c r="A83" s="21" t="s">
         <v>128</v>
       </c>
       <c r="B83" s="11"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="22" t="s">
+      <c r="A84" s="21" t="s">
         <v>129</v>
       </c>
       <c r="B84" s="11"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="22" t="s">
+      <c r="A85" s="21" t="s">
         <v>130</v>
       </c>
       <c r="B85" s="11"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="22" t="s">
+      <c r="A86" s="21" t="s">
         <v>131</v>
       </c>
       <c r="B86" s="11"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="22" t="s">
+      <c r="A87" s="21" t="s">
         <v>132</v>
       </c>
       <c r="B87" s="11"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="22" t="s">
+      <c r="A88" s="21" t="s">
         <v>133</v>
       </c>
       <c r="B88" s="11"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="s">
+      <c r="A89" s="21" t="s">
         <v>134</v>
       </c>
       <c r="B89" s="11"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="22" t="s">
+      <c r="A90" s="21" t="s">
         <v>135</v>
       </c>
       <c r="B90" s="11"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="22" t="s">
+      <c r="A91" s="21" t="s">
         <v>136</v>
       </c>
       <c r="B91" s="11"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="22" t="s">
+      <c r="A92" s="21" t="s">
         <v>137</v>
       </c>
       <c r="B92" s="11"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="22" t="s">
+      <c r="A93" s="21" t="s">
         <v>138</v>
       </c>
       <c r="B93" s="11"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="22" t="s">
+      <c r="A94" s="21" t="s">
         <v>139</v>
       </c>
       <c r="B94" s="11"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="22" t="s">
+      <c r="A95" s="21" t="s">
         <v>140</v>
       </c>
       <c r="B95" s="11"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="22" t="s">
+      <c r="A96" s="21" t="s">
         <v>141</v>
       </c>
       <c r="B96" s="11"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="22" t="s">
+      <c r="A97" s="21" t="s">
         <v>142</v>
       </c>
       <c r="B97" s="11"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="22" t="s">
+      <c r="A98" s="21" t="s">
         <v>143</v>
       </c>
       <c r="B98" s="11"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="22" t="s">
+      <c r="A99" s="21" t="s">
         <v>144</v>
       </c>
       <c r="B99" s="11"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="22" t="s">
+      <c r="A100" s="21" t="s">
         <v>145</v>
       </c>
       <c r="B100" s="11"/>

</xml_diff>